<commit_message>
uddated on 27th aug 2018
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>S.No</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>ssss</t>
+  </si>
+  <si>
+    <t>ffffff</t>
   </si>
 </sst>
 </file>
@@ -371,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -425,6 +428,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:5">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>234678902</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>